<commit_message>
push from pc 240826
</commit_message>
<xml_diff>
--- a/Put Portfolios/One Month_OnePointFive.xlsx
+++ b/Put Portfolios/One Month_OnePointFive.xlsx
@@ -469,16 +469,16 @@
         <v>20</v>
       </c>
       <c r="B2" t="n">
-        <v>-989436.730130323</v>
+        <v>-986487.1946236491</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>709318.0446234774</v>
+        <v>657686.8533694684</v>
       </c>
       <c r="E2" t="n">
-        <v>-280118.6855068456</v>
+        <v>-328800.3412541808</v>
       </c>
     </row>
     <row r="3">
@@ -486,16 +486,16 @@
         <v>21</v>
       </c>
       <c r="B3" t="n">
-        <v>-918762.6779781571</v>
+        <v>-917981.1394414512</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>638750.2175947312</v>
+        <v>590689.3819198005</v>
       </c>
       <c r="E3" t="n">
-        <v>-280012.4603834258</v>
+        <v>-327291.7575216506</v>
       </c>
     </row>
     <row r="4">
@@ -503,16 +503,16 @@
         <v>22</v>
       </c>
       <c r="B4" t="n">
-        <v>-848088.6258259912</v>
+        <v>-849475.0842592533</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>568389.5020042087</v>
+        <v>524818.941427311</v>
       </c>
       <c r="E4" t="n">
-        <v>-279699.1238217824</v>
+        <v>-324656.1428319423</v>
       </c>
     </row>
     <row r="5">
@@ -520,16 +520,16 @@
         <v>23</v>
       </c>
       <c r="B5" t="n">
-        <v>-777414.5736738251</v>
+        <v>-780969.0290770555</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>498508.7321681306</v>
+        <v>460589.6363104946</v>
       </c>
       <c r="E5" t="n">
-        <v>-278905.8415056946</v>
+        <v>-320379.392766561</v>
       </c>
     </row>
     <row r="6">
@@ -537,16 +537,16 @@
         <v>24</v>
       </c>
       <c r="B6" t="n">
-        <v>-706740.5215216592</v>
+        <v>-712462.9738948577</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>429591.2479875583</v>
+        <v>398589.3722152852</v>
       </c>
       <c r="E6" t="n">
-        <v>-277149.273534101</v>
+        <v>-313873.6016795725</v>
       </c>
     </row>
     <row r="7">
@@ -554,16 +554,16 @@
         <v>25</v>
       </c>
       <c r="B7" t="n">
-        <v>-636066.4693694933</v>
+        <v>-643956.9187126597</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>362375.2471930576</v>
+        <v>339435.6372968864</v>
       </c>
       <c r="E7" t="n">
-        <v>-273691.2221764358</v>
+        <v>-304521.2814157734</v>
       </c>
     </row>
     <row r="8">
@@ -571,16 +571,16 @@
         <v>26</v>
       </c>
       <c r="B8" t="n">
-        <v>-565392.4172173274</v>
+        <v>-575450.8635304619</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>297840.9424872215</v>
+        <v>283723.1279009996</v>
       </c>
       <c r="E8" t="n">
-        <v>-267551.4747301059</v>
+        <v>-291727.7356294623</v>
       </c>
     </row>
     <row r="9">
@@ -588,16 +588,16 @@
         <v>27</v>
       </c>
       <c r="B9" t="n">
-        <v>-494718.3650651615</v>
+        <v>-506944.8083482641</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>237123.5765046887</v>
+        <v>231972.3429270298</v>
       </c>
       <c r="E9" t="n">
-        <v>-257594.7885604728</v>
+        <v>-274972.4654212343</v>
       </c>
     </row>
     <row r="10">
@@ -605,16 +605,16 @@
         <v>28</v>
       </c>
       <c r="B10" t="n">
-        <v>-424044.3129129956</v>
+        <v>-438438.7531660662</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>181364.0953554639</v>
+        <v>184587.3746053973</v>
       </c>
       <c r="E10" t="n">
-        <v>-242680.2175575316</v>
+        <v>-253851.3785606689</v>
       </c>
     </row>
     <row r="11">
@@ -622,16 +622,16 @@
         <v>29</v>
       </c>
       <c r="B11" t="n">
-        <v>-353370.2607608296</v>
+        <v>-369932.6979838684</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>131535.8150110696</v>
+        <v>141828.4414078329</v>
       </c>
       <c r="E11" t="n">
-        <v>-221834.44574976</v>
+        <v>-228104.2565760355</v>
       </c>
     </row>
     <row r="12">
@@ -639,16 +639,16 @@
         <v>30</v>
       </c>
       <c r="B12" t="n">
-        <v>-282696.2086086637</v>
+        <v>-301426.6428016705</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>88295.6818569389</v>
+        <v>103801.2992957739</v>
       </c>
       <c r="E12" t="n">
-        <v>-194400.5267517248</v>
+        <v>-197625.3435058965</v>
       </c>
     </row>
     <row r="13">
@@ -656,16 +656,16 @@
         <v>31</v>
       </c>
       <c r="B13" t="n">
-        <v>-212022.1564564978</v>
+        <v>-232920.5876194726</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>51898.710469069</v>
+        <v>70462.51706227213</v>
       </c>
       <c r="E13" t="n">
-        <v>-160123.4459874288</v>
+        <v>-162458.0705572005</v>
       </c>
     </row>
     <row r="14">
@@ -673,16 +673,16 @@
         <v>32</v>
       </c>
       <c r="B14" t="n">
-        <v>-141348.1043043318</v>
+        <v>-164414.5324372748</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>22190.83919113178</v>
+        <v>41637.35145646712</v>
       </c>
       <c r="E14" t="n">
-        <v>-119157.2651132001</v>
+        <v>-122777.1809808076</v>
       </c>
     </row>
     <row r="15">
@@ -690,16 +690,16 @@
         <v>33</v>
       </c>
       <c r="B15" t="n">
-        <v>-70674.05215216592</v>
+        <v>-95908.47725507691</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-1329.254106355511</v>
+        <v>17045.83646943175</v>
       </c>
       <c r="E15" t="n">
-        <v>-72003.30625852144</v>
+        <v>-78862.64078564516</v>
       </c>
     </row>
     <row r="16">
@@ -707,16 +707,16 @@
         <v>34</v>
       </c>
       <c r="B16" t="n">
-        <v>0</v>
+        <v>-27402.42207287905</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-19405.18078266382</v>
+        <v>-3667.395361144643</v>
       </c>
       <c r="E16" t="n">
-        <v>-19405.18078266382</v>
+        <v>-31069.81743402369</v>
       </c>
     </row>
     <row r="17">
@@ -724,16 +724,16 @@
         <v>35</v>
       </c>
       <c r="B17" t="n">
-        <v>70674.05215216592</v>
+        <v>41103.63310931881</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-32904.95642498064</v>
+        <v>-20903.40610661578</v>
       </c>
       <c r="E17" t="n">
-        <v>37769.09572718529</v>
+        <v>20200.22700270303</v>
       </c>
     </row>
     <row r="18">
@@ -741,16 +741,16 @@
         <v>36</v>
       </c>
       <c r="B18" t="n">
-        <v>141348.1043043318</v>
+        <v>109609.6882915167</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-42715.10563521916</v>
+        <v>-35082.18205986936</v>
       </c>
       <c r="E18" t="n">
-        <v>98632.99866911268</v>
+        <v>74527.5062316473</v>
       </c>
     </row>
     <row r="19">
@@ -758,16 +758,16 @@
         <v>37</v>
       </c>
       <c r="B19" t="n">
-        <v>212022.1564564978</v>
+        <v>178115.7434737145</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-49661.46223179263</v>
+        <v>-46620.50701028899</v>
       </c>
       <c r="E19" t="n">
-        <v>162360.6942247052</v>
+        <v>131495.2364634256</v>
       </c>
     </row>
     <row r="20">
@@ -775,16 +775,16 @@
         <v>38</v>
       </c>
       <c r="B20" t="n">
-        <v>282696.2086086637</v>
+        <v>246621.7986559124</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-54461.04457016159</v>
+        <v>-55915.1890010403</v>
       </c>
       <c r="E20" t="n">
-        <v>228235.1640385021</v>
+        <v>190706.6096548721</v>
       </c>
     </row>
     <row r="21">
@@ -792,16 +792,16 @@
         <v>39</v>
       </c>
       <c r="B21" t="n">
-        <v>353370.2607608296</v>
+        <v>315127.8538381102</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-57701.83465806887</v>
+        <v>-63331.58105176363</v>
       </c>
       <c r="E21" t="n">
-        <v>295668.4261027607</v>
+        <v>251796.2727863466</v>
       </c>
     </row>
     <row r="22">
@@ -809,16 +809,16 @@
         <v>40</v>
       </c>
       <c r="B22" t="n">
-        <v>424044.3129129956</v>
+        <v>383633.9090203081</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-59843.37276359624</v>
+        <v>-69196.82599906511</v>
       </c>
       <c r="E22" t="n">
-        <v>364200.9401493993</v>
+        <v>314437.083021243</v>
       </c>
     </row>
     <row r="23">
@@ -826,16 +826,16 @@
         <v>41</v>
       </c>
       <c r="B23" t="n">
-        <v>494718.3650651615</v>
+        <v>452139.9642025059</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-61230.24276751895</v>
+        <v>-73796.98200809315</v>
       </c>
       <c r="E23" t="n">
-        <v>433488.1222976425</v>
+        <v>378342.9821944128</v>
       </c>
     </row>
     <row r="24">
@@ -843,16 +843,16 @@
         <v>42</v>
       </c>
       <c r="B24" t="n">
-        <v>565392.4172173274</v>
+        <v>520646.0193847038</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-62111.62417467596</v>
+        <v>-77377.09853698111</v>
       </c>
       <c r="E24" t="n">
-        <v>503280.7930426514</v>
+        <v>443268.9208477227</v>
       </c>
     </row>
     <row r="25">
@@ -860,16 +860,16 @@
         <v>43</v>
       </c>
       <c r="B25" t="n">
-        <v>636066.4693694933</v>
+        <v>589152.0745669017</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-62662.00784130788</v>
+        <v>-80143.35479058795</v>
       </c>
       <c r="E25" t="n">
-        <v>573404.4615281854</v>
+        <v>509008.7197763137</v>
       </c>
     </row>
     <row r="26">
@@ -877,16 +877,16 @@
         <v>44</v>
       </c>
       <c r="B26" t="n">
-        <v>706740.5215216592</v>
+        <v>657658.1297490995</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-63000.12450865044</v>
+        <v>-82266.49083529468</v>
       </c>
       <c r="E26" t="n">
-        <v>643740.3970130088</v>
+        <v>575391.6389138048</v>
       </c>
     </row>
     <row r="27">
@@ -894,16 +894,16 @@
         <v>45</v>
       </c>
       <c r="B27" t="n">
-        <v>777414.5736738251</v>
+        <v>726164.1849312974</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-63204.70437016525</v>
+        <v>-83885.91330745442</v>
       </c>
       <c r="E27" t="n">
-        <v>714209.8693036599</v>
+        <v>642278.271623843</v>
       </c>
     </row>
   </sheetData>
@@ -957,16 +957,16 @@
         <v>30</v>
       </c>
       <c r="B2" t="n">
-        <v>-1009921.962638197</v>
+        <v>-1059392.721239566</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>678186.530373562</v>
+        <v>678709.7445565411</v>
       </c>
       <c r="E2" t="n">
-        <v>-331735.4322646351</v>
+        <v>-380682.976683025</v>
       </c>
     </row>
     <row r="3">
@@ -974,16 +974,16 @@
         <v>31</v>
       </c>
       <c r="B3" t="n">
-        <v>-963488.7689536823</v>
+        <v>-1016152.202005298</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>632324.8192075271</v>
+        <v>637252.0397436456</v>
       </c>
       <c r="E3" t="n">
-        <v>-331163.9497461552</v>
+        <v>-378900.1622616525</v>
       </c>
     </row>
     <row r="4">
@@ -991,16 +991,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="n">
-        <v>-917055.5752691675</v>
+        <v>-972911.6827710301</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>586779.1352299097</v>
+        <v>596340.3363777321</v>
       </c>
       <c r="E4" t="n">
-        <v>-330276.4400392579</v>
+        <v>-376571.346393298</v>
       </c>
     </row>
     <row r="5">
@@ -1008,16 +1008,16 @@
         <v>33</v>
       </c>
       <c r="B5" t="n">
-        <v>-870622.3815846527</v>
+        <v>-929671.1635367621</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>541670.6464692074</v>
+        <v>556076.3886625431</v>
       </c>
       <c r="E5" t="n">
-        <v>-328951.7351154453</v>
+        <v>-373594.774874219</v>
       </c>
     </row>
     <row r="6">
@@ -1025,16 +1025,16 @@
         <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>-824189.1879001379</v>
+        <v>-886430.6443024941</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>497144.3749782451</v>
+        <v>516565.4266703369</v>
       </c>
       <c r="E6" t="n">
-        <v>-327044.8129218928</v>
+        <v>-369865.2176321572</v>
       </c>
     </row>
     <row r="7">
@@ -1042,16 +1042,16 @@
         <v>35</v>
       </c>
       <c r="B7" t="n">
-        <v>-777755.994215623</v>
+        <v>-843190.1250682261</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>453366.7626986392</v>
+        <v>477913.5510296458</v>
       </c>
       <c r="E7" t="n">
-        <v>-324389.2315169838</v>
+        <v>-365276.5740385804</v>
       </c>
     </row>
     <row r="8">
@@ -1059,16 +1059,16 @@
         <v>36</v>
       </c>
       <c r="B8" t="n">
-        <v>-731322.8005311083</v>
+        <v>-799949.6058339581</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>410521.2662422417</v>
+        <v>440225.0724594775</v>
       </c>
       <c r="E8" t="n">
-        <v>-320801.5342888666</v>
+        <v>-359724.5333744807</v>
       </c>
     </row>
     <row r="9">
@@ -1076,16 +1076,16 @@
         <v>37</v>
       </c>
       <c r="B9" t="n">
-        <v>-684889.6068465934</v>
+        <v>-756709.08659969</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>368802.2465194969</v>
+        <v>403599.9348245525</v>
       </c>
       <c r="E9" t="n">
-        <v>-316087.3603270965</v>
+        <v>-353109.1517751375</v>
       </c>
     </row>
     <row r="10">
@@ -1093,16 +1093,16 @@
         <v>38</v>
       </c>
       <c r="B10" t="n">
-        <v>-638456.4131620786</v>
+        <v>-713468.5673654221</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>328407.6231760796</v>
+        <v>368131.3429063596</v>
       </c>
       <c r="E10" t="n">
-        <v>-310048.789985999</v>
+        <v>-345337.2244590626</v>
       </c>
     </row>
     <row r="11">
@@ -1110,16 +1110,16 @@
         <v>39</v>
       </c>
       <c r="B11" t="n">
-        <v>-592023.2194775639</v>
+        <v>-670228.048131154</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>289530.8981785898</v>
+        <v>333903.6919565909</v>
       </c>
       <c r="E11" t="n">
-        <v>-302492.321298974</v>
+        <v>-336324.3561745632</v>
       </c>
     </row>
     <row r="12">
@@ -1127,16 +1127,16 @@
         <v>40</v>
       </c>
       <c r="B12" t="n">
-        <v>-545590.025793049</v>
+        <v>-626987.5288968862</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>252353.2029375672</v>
+        <v>300990.8684947646</v>
       </c>
       <c r="E12" t="n">
-        <v>-293236.8228554819</v>
+        <v>-325996.6604021216</v>
       </c>
     </row>
     <row r="13">
@@ -1144,16 +1144,16 @@
         <v>41</v>
       </c>
       <c r="B13" t="n">
-        <v>-499156.8321085342</v>
+        <v>-583747.009662618</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>217035.9903511704</v>
+        <v>269454.9635728811</v>
       </c>
       <c r="E13" t="n">
-        <v>-282120.8417573638</v>
+        <v>-314292.046089737</v>
       </c>
     </row>
     <row r="14">
@@ -1161,16 +1161,16 @@
         <v>42</v>
       </c>
       <c r="B14" t="n">
-        <v>-452723.6384240194</v>
+        <v>-540506.4904283501</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>183714.8914109238</v>
+        <v>239345.4131518628</v>
       </c>
       <c r="E14" t="n">
-        <v>-269008.7470130956</v>
+        <v>-301161.0772764873</v>
       </c>
     </row>
     <row r="15">
@@ -1178,16 +1178,16 @@
         <v>43</v>
       </c>
       <c r="B15" t="n">
-        <v>-406290.4447395046</v>
+        <v>-497265.9711940821</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>152495.1080099572</v>
+        <v>210698.5569697243</v>
       </c>
       <c r="E15" t="n">
-        <v>-253795.3367295474</v>
+        <v>-286567.4142243578</v>
       </c>
     </row>
     <row r="16">
@@ -1195,16 +1195,16 @@
         <v>44</v>
       </c>
       <c r="B16" t="n">
-        <v>-359857.2510549898</v>
+        <v>-454025.4519598141</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>123448.5446463842</v>
+        <v>183537.5883410708</v>
       </c>
       <c r="E16" t="n">
-        <v>-236408.7064086056</v>
+        <v>-270487.8636187433</v>
       </c>
     </row>
     <row r="17">
@@ -1212,16 +1212,16 @@
         <v>45</v>
       </c>
       <c r="B17" t="n">
-        <v>-313424.057370475</v>
+        <v>-410784.9327255461</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>96612.7153640558</v>
+        <v>157872.8531501832</v>
       </c>
       <c r="E17" t="n">
-        <v>-216811.3420064192</v>
+        <v>-252912.0795753628</v>
       </c>
     </row>
     <row r="18">
@@ -1229,16 +1229,16 @@
         <v>46</v>
       </c>
       <c r="B18" t="n">
-        <v>-266990.8636859602</v>
+        <v>-367544.4134912781</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>71991.31710881696</v>
+        <v>133702.4468582718</v>
       </c>
       <c r="E18" t="n">
-        <v>-194999.5465771432</v>
+        <v>-233841.9666330063</v>
       </c>
     </row>
     <row r="19">
@@ -1246,16 +1246,16 @@
         <v>47</v>
       </c>
       <c r="B19" t="n">
-        <v>-220557.6700014453</v>
+        <v>-324303.89425701</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>49556.24876129536</v>
+        <v>111013.0532686702</v>
       </c>
       <c r="E19" t="n">
-        <v>-171001.42124015</v>
+        <v>-213290.8409883399</v>
       </c>
     </row>
     <row r="20">
@@ -1263,16 +1263,16 @@
         <v>48</v>
       </c>
       <c r="B20" t="n">
-        <v>-174124.4763169306</v>
+        <v>-281063.375022742</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>29250.78183407447</v>
+        <v>89780.9674866023</v>
       </c>
       <c r="E20" t="n">
-        <v>-144873.6944828561</v>
+        <v>-191282.4075361397</v>
       </c>
     </row>
     <row r="21">
@@ -1280,16 +1280,16 @@
         <v>49</v>
       </c>
       <c r="B21" t="n">
-        <v>-127691.2826324157</v>
+        <v>-237822.855788474</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>10993.55383567831</v>
+        <v>69973.24725895248</v>
       </c>
       <c r="E21" t="n">
-        <v>-116697.7287967374</v>
+        <v>-167849.6085295216</v>
       </c>
     </row>
     <row r="22">
@@ -1297,16 +1297,16 @@
         <v>50</v>
       </c>
       <c r="B22" t="n">
-        <v>-81258.08894790092</v>
+        <v>-194582.336554206</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-5316.94600321955</v>
+        <v>51548.94093737979</v>
       </c>
       <c r="E22" t="n">
-        <v>-86575.03495112047</v>
+        <v>-143033.3956168262</v>
       </c>
     </row>
     <row r="23">
@@ -1314,16 +1314,16 @@
         <v>51</v>
       </c>
       <c r="B23" t="n">
-        <v>-34824.8952633861</v>
+        <v>-151341.817319938</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-19797.70375930217</v>
+        <v>34460.34595901366</v>
       </c>
       <c r="E23" t="n">
-        <v>-54622.59902268827</v>
+        <v>-116881.4713609244</v>
       </c>
     </row>
     <row r="24">
@@ -1331,16 +1331,16 @@
         <v>52</v>
       </c>
       <c r="B24" t="n">
-        <v>11608.2984211287</v>
+        <v>-108101.29808567</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-32576.58225350467</v>
+        <v>18654.25834047099</v>
       </c>
       <c r="E24" t="n">
-        <v>-20968.28383237597</v>
+        <v>-89447.039745199</v>
       </c>
     </row>
     <row r="25">
@@ -1348,16 +1348,16 @@
         <v>53</v>
       </c>
       <c r="B25" t="n">
-        <v>58041.49210564351</v>
+        <v>-64860.77885140201</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-43788.00481291229</v>
+        <v>4073.180688950687</v>
       </c>
       <c r="E25" t="n">
-        <v>14253.48729273122</v>
+        <v>-60787.59816245133</v>
       </c>
     </row>
     <row r="26">
@@ -1365,16 +1365,16 @@
         <v>54</v>
       </c>
       <c r="B26" t="n">
-        <v>104474.6857901583</v>
+        <v>-21620.259617134</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-53569.072241908</v>
+        <v>-9343.536786745515</v>
       </c>
       <c r="E26" t="n">
-        <v>50905.61354825033</v>
+        <v>-30963.79640387952</v>
       </c>
     </row>
     <row r="27">
@@ -1382,16 +1382,16 @@
         <v>55</v>
       </c>
       <c r="B27" t="n">
-        <v>150907.8794746731</v>
+        <v>21620.259617134</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-62056.2090172918</v>
+        <v>-21658.64116006315</v>
       </c>
       <c r="E27" t="n">
-        <v>88851.67045738133</v>
+        <v>-38.38154292915351</v>
       </c>
     </row>
     <row r="28">
@@ -1399,16 +1399,16 @@
         <v>56</v>
       </c>
       <c r="B28" t="n">
-        <v>197341.0731591879</v>
+        <v>64860.77885140201</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-69382.38583073203</v>
+        <v>-32936.02042273077</v>
       </c>
       <c r="E28" t="n">
-        <v>127958.6873284559</v>
+        <v>31924.75842867124</v>
       </c>
     </row>
     <row r="29">
@@ -1416,16 +1416,16 @@
         <v>57</v>
       </c>
       <c r="B29" t="n">
-        <v>243774.2668437028</v>
+        <v>108101.29808567</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-75674.9249430746</v>
+        <v>-43239.85341919394</v>
       </c>
       <c r="E29" t="n">
-        <v>168099.3419006282</v>
+        <v>64861.44466647606</v>
       </c>
     </row>
     <row r="30">
@@ -1433,16 +1433,16 @@
         <v>58</v>
       </c>
       <c r="B30" t="n">
-        <v>290207.4605282175</v>
+        <v>151341.817319938</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-81053.86331725107</v>
+        <v>-52633.8691103732</v>
       </c>
       <c r="E30" t="n">
-        <v>209153.5972109665</v>
+        <v>98707.94820956484</v>
       </c>
     </row>
     <row r="31">
@@ -1450,16 +1450,16 @@
         <v>59</v>
       </c>
       <c r="B31" t="n">
-        <v>336640.6542127323</v>
+        <v>194582.336554206</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-85630.82606558251</v>
+        <v>-61180.71449112163</v>
       </c>
       <c r="E31" t="n">
-        <v>251009.8281471498</v>
+        <v>133401.6220630844</v>
       </c>
     </row>
     <row r="32">
@@ -1467,16 +1467,16 @@
         <v>60</v>
       </c>
       <c r="B32" t="n">
-        <v>383073.8478972472</v>
+        <v>237822.855788474</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-89508.34857998797</v>
+        <v>-68941.42755852931</v>
       </c>
       <c r="E32" t="n">
-        <v>293565.4993172592</v>
+        <v>168881.4282299447</v>
       </c>
     </row>
     <row r="33">
@@ -1484,16 +1484,16 @@
         <v>61</v>
       </c>
       <c r="B33" t="n">
-        <v>429507.041581762</v>
+        <v>281063.375022742</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>-92779.57858336078</v>
+        <v>-75975.00952166095</v>
       </c>
       <c r="E33" t="n">
-        <v>336727.4629984012</v>
+        <v>205088.3655010811</v>
       </c>
     </row>
     <row r="34">
@@ -1501,16 +1501,16 @@
         <v>62</v>
       </c>
       <c r="B34" t="n">
-        <v>475940.2352662768</v>
+        <v>324303.89425701</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>-95528.28783258564</v>
+        <v>-82338.08888033086</v>
       </c>
       <c r="E34" t="n">
-        <v>380411.9474336911</v>
+        <v>241965.8053766792</v>
       </c>
     </row>
     <row r="35">
@@ -1518,16 +1518,16 @@
         <v>63</v>
       </c>
       <c r="B35" t="n">
-        <v>522373.4289507916</v>
+        <v>367544.4134912781</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>-97829.12589330049</v>
+        <v>-88084.66899444503</v>
       </c>
       <c r="E35" t="n">
-        <v>424544.3030574911</v>
+        <v>279459.7444968331</v>
       </c>
     </row>
     <row r="36">
@@ -1535,16 +1535,16 @@
         <v>64</v>
       </c>
       <c r="B36" t="n">
-        <v>568806.6226353064</v>
+        <v>410784.9327255461</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>-99748.05397875293</v>
+        <v>-93265.95022700851</v>
       </c>
       <c r="E36" t="n">
-        <v>469058.5686565535</v>
+        <v>317518.9824985376</v>
       </c>
     </row>
     <row r="37">
@@ -1552,16 +1552,16 @@
         <v>65</v>
       </c>
       <c r="B37" t="n">
-        <v>615239.8163198213</v>
+        <v>454025.4519598141</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>-101342.9041669213</v>
+        <v>-97930.21758612921</v>
       </c>
       <c r="E37" t="n">
-        <v>513896.9121529</v>
+        <v>356095.2343736849</v>
       </c>
     </row>
     <row r="38">
@@ -1569,16 +1569,16 @@
         <v>66</v>
       </c>
       <c r="B38" t="n">
-        <v>661673.010004336</v>
+        <v>497265.9711940821</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>-102664.017462144</v>
+        <v>-102122.7849331375</v>
       </c>
       <c r="E38" t="n">
-        <v>559008.992542192</v>
+        <v>395143.1862609446</v>
       </c>
     </row>
     <row r="39">
@@ -1586,16 +1586,16 @@
         <v>67</v>
       </c>
       <c r="B39" t="n">
-        <v>708106.2036888509</v>
+        <v>540506.4904283501</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>-103754.9224473696</v>
+        <v>-105885.9871922547</v>
       </c>
       <c r="E39" t="n">
-        <v>604351.2812414812</v>
+        <v>434620.5032360954</v>
       </c>
     </row>
     <row r="40">
@@ -1603,16 +1603,16 @@
         <v>68</v>
       </c>
       <c r="B40" t="n">
-        <v>754539.3973733657</v>
+        <v>583747.009662618</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>-104653.024179318</v>
+        <v>-109259.2125281388</v>
       </c>
       <c r="E40" t="n">
-        <v>649886.3731940477</v>
+        <v>474487.7971344792</v>
       </c>
     </row>
     <row r="41">
@@ -1620,16 +1620,16 @@
         <v>69</v>
       </c>
       <c r="B41" t="n">
-        <v>800972.5910578805</v>
+        <v>626987.5288968862</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>-105390.2801836059</v>
+        <v>-112278.967096824</v>
       </c>
       <c r="E41" t="n">
-        <v>695582.3108742746</v>
+        <v>514708.5618000621</v>
       </c>
     </row>
     <row r="42">
@@ -1637,16 +1637,16 @@
         <v>70</v>
       </c>
       <c r="B42" t="n">
-        <v>847405.7847423953</v>
+        <v>670228.048131154</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>-105993.8467244827</v>
+        <v>-114978.9656780087</v>
       </c>
       <c r="E42" t="n">
-        <v>741411.9380179126</v>
+        <v>555249.0824531453</v>
       </c>
     </row>
     <row r="43">
@@ -1654,16 +1654,16 @@
         <v>71</v>
       </c>
       <c r="B43" t="n">
-        <v>893838.97842691</v>
+        <v>713468.5673654221</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>-106486.6838782105</v>
+        <v>-117390.2422261676</v>
       </c>
       <c r="E43" t="n">
-        <v>787352.2945486995</v>
+        <v>596078.3251392546</v>
       </c>
     </row>
     <row r="44">
@@ -1671,16 +1671,16 @@
         <v>72</v>
       </c>
       <c r="B44" t="n">
-        <v>940272.172111425</v>
+        <v>756709.08659969</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>-106888.1123341149</v>
+        <v>-119541.2751062179</v>
       </c>
       <c r="E44" t="n">
-        <v>833384.05977731</v>
+        <v>637167.8114934721</v>
       </c>
     </row>
     <row r="45">
@@ -1688,16 +1688,16 @@
         <v>73</v>
       </c>
       <c r="B45" t="n">
-        <v>986705.3657959397</v>
+        <v>799949.6058339581</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>-107214.3183408402</v>
+        <v>-121458.1224851773</v>
       </c>
       <c r="E45" t="n">
-        <v>879491.0474550994</v>
+        <v>678491.4833487808</v>
       </c>
     </row>
     <row r="46">
@@ -1705,16 +1705,16 @@
         <v>74</v>
       </c>
       <c r="B46" t="n">
-        <v>1033138.559480454</v>
+        <v>843190.1250682261</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>-107478.8058984699</v>
+        <v>-123164.5640190764</v>
       </c>
       <c r="E46" t="n">
-        <v>925659.7535819844</v>
+        <v>720025.5610491497</v>
       </c>
     </row>
     <row r="47">
@@ -1722,16 +1722,16 @@
         <v>75</v>
       </c>
       <c r="B47" t="n">
-        <v>1079571.753164969</v>
+        <v>886430.6443024941</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>-107692.7972777204</v>
+        <v>-124682.2455939589</v>
       </c>
       <c r="E47" t="n">
-        <v>971878.955887249</v>
+        <v>761748.3987085352</v>
       </c>
     </row>
     <row r="48">
@@ -1739,16 +1739,16 @@
         <v>76</v>
       </c>
       <c r="B48" t="n">
-        <v>1126004.946849484</v>
+        <v>929671.1635367621</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>-107865.5843380098</v>
+        <v>-126030.8244449508</v>
       </c>
       <c r="E48" t="n">
-        <v>1018139.362511474</v>
+        <v>803640.3390918113</v>
       </c>
     </row>
     <row r="49">
@@ -1756,16 +1756,16 @@
         <v>77</v>
       </c>
       <c r="B49" t="n">
-        <v>1172438.140533999</v>
+        <v>972911.6827710301</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>-108004.8340259723</v>
+        <v>-127228.1124849806</v>
       </c>
       <c r="E49" t="n">
-        <v>1064433.306508027</v>
+        <v>845683.5702860495</v>
       </c>
     </row>
     <row r="50">
@@ -1773,16 +1773,16 @@
         <v>78</v>
       </c>
       <c r="B50" t="n">
-        <v>1218871.334218514</v>
+        <v>1016152.202005298</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>-108116.8519652528</v>
+        <v>-128290.2161244259</v>
       </c>
       <c r="E50" t="n">
-        <v>1110754.482253261</v>
+        <v>887861.9858808722</v>
       </c>
     </row>
     <row r="51">
@@ -1790,16 +1790,16 @@
         <v>79</v>
       </c>
       <c r="B51" t="n">
-        <v>1265304.527903029</v>
+        <v>1059392.721239566</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>-108206.808285813</v>
+        <v>-129231.6712560418</v>
       </c>
       <c r="E51" t="n">
-        <v>1157097.719617215</v>
+        <v>930161.0499835243</v>
       </c>
     </row>
     <row r="52">
@@ -1807,16 +1807,16 @@
         <v>80</v>
       </c>
       <c r="B52" t="n">
-        <v>1311737.721587543</v>
+        <v>1102633.240473834</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>-108278.9298622079</v>
+        <v>-130065.5724187794</v>
       </c>
       <c r="E52" t="n">
-        <v>1203458.791725335</v>
+        <v>972567.6680550547</v>
       </c>
     </row>
     <row r="53">
@@ -1824,16 +1824,16 @@
         <v>81</v>
       </c>
       <c r="B53" t="n">
-        <v>1358170.915272058</v>
+        <v>1145873.759708102</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>-108336.6629981437</v>
+        <v>-130803.6954431659</v>
       </c>
       <c r="E53" t="n">
-        <v>1249834.252273914</v>
+        <v>1015070.064264936</v>
       </c>
     </row>
     <row r="54">
@@ -1841,16 +1841,16 @@
         <v>82</v>
       </c>
       <c r="B54" t="n">
-        <v>1404604.108956573</v>
+        <v>1189114.27894237</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>-108382.8103597614</v>
+        <v>-131456.6131239919</v>
       </c>
       <c r="E54" t="n">
-        <v>1296221.298596812</v>
+        <v>1057657.665818378</v>
       </c>
     </row>
     <row r="55">
@@ -1858,16 +1858,16 @@
         <v>83</v>
       </c>
       <c r="B55" t="n">
-        <v>1451037.302641088</v>
+        <v>1232354.798176638</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>-108419.6456622504</v>
+        <v>-132033.8036676166</v>
       </c>
       <c r="E55" t="n">
-        <v>1342617.656978837</v>
+        <v>1100320.994509022</v>
       </c>
     </row>
     <row r="56">
@@ -1875,16 +1875,16 @@
         <v>84</v>
       </c>
       <c r="B56" t="n">
-        <v>1497470.496325603</v>
+        <v>1275595.317410906</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>-108449.0092839337</v>
+        <v>-132543.75182582</v>
       </c>
       <c r="E56" t="n">
-        <v>1389021.487041669</v>
+        <v>1143051.565585086</v>
       </c>
     </row>
     <row r="57">
@@ -1892,16 +1892,16 @@
         <v>85</v>
       </c>
       <c r="B57" t="n">
-        <v>1543903.690010117</v>
+        <v>1318835.836645174</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>-108472.3876412419</v>
+        <v>-132994.0427602539</v>
       </c>
       <c r="E57" t="n">
-        <v>1435431.302368875</v>
+        <v>1185841.79388492</v>
       </c>
     </row>
     <row r="58">
@@ -1909,16 +1909,16 @@
         <v>86</v>
       </c>
       <c r="B58" t="n">
-        <v>1590336.883694632</v>
+        <v>1362076.355879442</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>-108490.9788229574</v>
+        <v>-133391.4487854092</v>
       </c>
       <c r="E58" t="n">
-        <v>1481845.904871675</v>
+        <v>1228684.907094033</v>
       </c>
     </row>
     <row r="59">
@@ -1926,16 +1926,16 @@
         <v>87</v>
       </c>
       <c r="B59" t="n">
-        <v>1636770.077379147</v>
+        <v>1405316.87511371</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>-108505.7466634616</v>
+        <v>-133742.0092176333</v>
       </c>
       <c r="E59" t="n">
-        <v>1528264.330715685</v>
+        <v>1271574.865896077</v>
       </c>
     </row>
     <row r="60">
@@ -1943,16 +1943,16 @@
         <v>88</v>
       </c>
       <c r="B60" t="n">
-        <v>1683203.271063662</v>
+        <v>1448557.394347978</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>-108517.4651392252</v>
+        <v>-134051.1036167216</v>
       </c>
       <c r="E60" t="n">
-        <v>1574685.805924437</v>
+        <v>1314506.290731256</v>
       </c>
     </row>
     <row r="61">
@@ -1960,16 +1960,16 @@
         <v>89</v>
       </c>
       <c r="B61" t="n">
-        <v>1729636.464748177</v>
+        <v>1491797.913582246</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>-108526.754704097</v>
+        <v>-134323.5187482827</v>
       </c>
       <c r="E61" t="n">
-        <v>1621109.71004408</v>
+        <v>1357474.394833964</v>
       </c>
     </row>
     <row r="62">
@@ -1977,16 +1977,16 @@
         <v>90</v>
       </c>
       <c r="B62" t="n">
-        <v>1776069.658432692</v>
+        <v>1535038.432816514</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>-108534.1119385533</v>
+        <v>-134563.5096223971</v>
       </c>
       <c r="E62" t="n">
-        <v>1667535.546494138</v>
+        <v>1400474.923194117</v>
       </c>
     </row>
   </sheetData>
@@ -2040,16 +2040,16 @@
         <v>30</v>
       </c>
       <c r="B2" t="n">
-        <v>-1306195.831971614</v>
+        <v>-1354932.909375169</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>1010680.882350679</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-295514.9496209351</v>
+        <v>-1354932.909375169</v>
       </c>
     </row>
     <row r="3">
@@ -2057,16 +2057,16 @@
         <v>31</v>
       </c>
       <c r="B3" t="n">
-        <v>-1269638.433931547</v>
+        <v>-1321543.729745422</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>974335.0547634372</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-295303.3791681095</v>
+        <v>-1321543.729745422</v>
       </c>
     </row>
     <row r="4">
@@ -2074,16 +2074,16 @@
         <v>32</v>
       </c>
       <c r="B4" t="n">
-        <v>-1233081.035891479</v>
+        <v>-1288154.550115674</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>937989.4347576416</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-295091.6011338377</v>
+        <v>-1288154.550115674</v>
       </c>
     </row>
     <row r="5">
@@ -2091,16 +2091,16 @@
         <v>33</v>
       </c>
       <c r="B5" t="n">
-        <v>-1196523.637851412</v>
+        <v>-1254765.370485926</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>901644.3163267833</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-294879.3215246284</v>
+        <v>-1254765.370485926</v>
       </c>
     </row>
     <row r="6">
@@ -2108,16 +2108,16 @@
         <v>34</v>
       </c>
       <c r="B6" t="n">
-        <v>-1159966.239811344</v>
+        <v>-1221376.190856178</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>865300.327841638</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-294665.9119697061</v>
+        <v>-1221376.190856178</v>
       </c>
     </row>
     <row r="7">
@@ -2125,16 +2125,16 @@
         <v>35</v>
       </c>
       <c r="B7" t="n">
-        <v>-1123408.841771276</v>
+        <v>-1187987.01122643</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>828958.7253390762</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-294450.1164322002</v>
+        <v>-1187987.01122643</v>
       </c>
     </row>
     <row r="8">
@@ -2142,16 +2142,16 @@
         <v>36</v>
       </c>
       <c r="B8" t="n">
-        <v>-1086851.443731209</v>
+        <v>-1154597.831596682</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>792621.8680314376</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-294229.5756997712</v>
+        <v>-1154597.831596682</v>
       </c>
     </row>
     <row r="9">
@@ -2159,16 +2159,16 @@
         <v>37</v>
       </c>
       <c r="B9" t="n">
-        <v>-1050294.045691141</v>
+        <v>-1121208.651966934</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>756293.9378029533</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-294000.1078881879</v>
+        <v>-1121208.651966934</v>
       </c>
     </row>
     <row r="10">
@@ -2176,16 +2176,16 @@
         <v>38</v>
       </c>
       <c r="B10" t="n">
-        <v>-1013736.647651074</v>
+        <v>-1087819.472337186</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>719981.9571774531</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-293754.6904736208</v>
+        <v>-1087819.472337186</v>
       </c>
     </row>
     <row r="11">
@@ -2193,16 +2193,16 @@
         <v>39</v>
       </c>
       <c r="B11" t="n">
-        <v>-977179.2496110062</v>
+        <v>-1054430.292707438</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>683697.1370108055</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-293482.1126002007</v>
+        <v>-1054430.292707438</v>
       </c>
     </row>
     <row r="12">
@@ -2210,16 +2210,16 @@
         <v>40</v>
       </c>
       <c r="B12" t="n">
-        <v>-940621.8515709386</v>
+        <v>-1021041.11307769</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>647456.5445812301</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-293165.3069897084</v>
+        <v>-1021041.11307769</v>
       </c>
     </row>
     <row r="13">
@@ -2227,16 +2227,16 @@
         <v>41</v>
       </c>
       <c r="B13" t="n">
-        <v>-904064.4535308711</v>
+        <v>-987651.9334479426</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>611285.027546151</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>-292779.4259847201</v>
+        <v>-987651.9334479426</v>
       </c>
     </row>
     <row r="14">
@@ -2244,16 +2244,16 @@
         <v>42</v>
       </c>
       <c r="B14" t="n">
-        <v>-867507.0554908034</v>
+        <v>-954262.7538181947</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>575217.2666285299</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>-292289.7888622736</v>
+        <v>-954262.7538181947</v>
       </c>
     </row>
     <row r="15">
@@ -2261,16 +2261,16 @@
         <v>43</v>
       </c>
       <c r="B15" t="n">
-        <v>-830949.6574507359</v>
+        <v>-920873.5741884467</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>539299.7706853686</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>-291649.8867653674</v>
+        <v>-920873.5741884467</v>
       </c>
     </row>
     <row r="16">
@@ -2278,16 +2278,16 @@
         <v>44</v>
       </c>
       <c r="B16" t="n">
-        <v>-794392.2594106684</v>
+        <v>-887484.3945586988</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>503592.5842612081</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>-290799.6751494603</v>
+        <v>-887484.3945586988</v>
       </c>
     </row>
     <row r="17">
@@ -2295,16 +2295,16 @@
         <v>45</v>
       </c>
       <c r="B17" t="n">
-        <v>-757834.8613706008</v>
+        <v>-854095.214928951</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>468170.4608056712</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>-289664.4005649295</v>
+        <v>-854095.214928951</v>
       </c>
     </row>
     <row r="18">
@@ -2312,16 +2312,16 @@
         <v>46</v>
       </c>
       <c r="B18" t="n">
-        <v>-721277.4633305332</v>
+        <v>-820706.0352992031</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>433123.2714305734</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>-288154.1918999599</v>
+        <v>-820706.0352992031</v>
       </c>
     </row>
     <row r="19">
@@ -2329,16 +2329,16 @@
         <v>47</v>
       </c>
       <c r="B19" t="n">
-        <v>-684720.0652904657</v>
+        <v>-787316.8556694551</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>398555.4705838589</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>-286164.5947066068</v>
+        <v>-787316.8556694551</v>
       </c>
     </row>
     <row r="20">
@@ -2346,16 +2346,16 @@
         <v>48</v>
       </c>
       <c r="B20" t="n">
-        <v>-648162.6672503981</v>
+        <v>-753927.6760397073</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>364584.5211853266</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>-283578.1460650715</v>
+        <v>-753927.6760397073</v>
       </c>
     </row>
     <row r="21">
@@ -2363,16 +2363,16 @@
         <v>49</v>
       </c>
       <c r="B21" t="n">
-        <v>-611605.2692103304</v>
+        <v>-720538.4964099595</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>331338.2820476835</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>-280266.987162647</v>
+        <v>-720538.4964099595</v>
       </c>
     </row>
     <row r="22">
@@ -2380,16 +2380,16 @@
         <v>50</v>
       </c>
       <c r="B22" t="n">
-        <v>-575047.871170263</v>
+        <v>-687149.3167802115</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>298951.4658771792</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>-276096.4052930839</v>
+        <v>-687149.3167802115</v>
       </c>
     </row>
     <row r="23">
@@ -2397,16 +2397,16 @@
         <v>51</v>
       </c>
       <c r="B23" t="n">
-        <v>-538490.4731301954</v>
+        <v>-653760.1371504636</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>267561.3721756301</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>-270929.1009545653</v>
+        <v>-653760.1371504636</v>
       </c>
     </row>
     <row r="24">
@@ -2414,16 +2414,16 @@
         <v>52</v>
       </c>
       <c r="B24" t="n">
-        <v>-501933.0750901279</v>
+        <v>-620370.9575207158</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>237303.173207657</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>-264629.9018824709</v>
+        <v>-620370.9575207158</v>
       </c>
     </row>
     <row r="25">
@@ -2431,16 +2431,16 @@
         <v>53</v>
       </c>
       <c r="B25" t="n">
-        <v>-465375.6770500603</v>
+        <v>-586981.7778909679</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>208305.0740275347</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>-257070.6030225256</v>
+        <v>-586981.7778909679</v>
       </c>
     </row>
     <row r="26">
@@ -2448,16 +2448,16 @@
         <v>54</v>
       </c>
       <c r="B26" t="n">
-        <v>-428818.2790099927</v>
+        <v>-553592.5982612199</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>180683.6755684374</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>-248134.6034415553</v>
+        <v>-553592.5982612199</v>
       </c>
     </row>
     <row r="27">
@@ -2465,16 +2465,16 @@
         <v>55</v>
       </c>
       <c r="B27" t="n">
-        <v>-392260.8809699251</v>
+        <v>-520203.4186314721</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>154539.8442741239</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>-237721.0366958012</v>
+        <v>-520203.4186314721</v>
       </c>
     </row>
     <row r="28">
@@ -2482,16 +2482,16 @@
         <v>56</v>
       </c>
       <c r="B28" t="n">
-        <v>-355703.4829298576</v>
+        <v>-486814.2390017241</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>129955.3383035563</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>-225748.1446263012</v>
+        <v>-486814.2390017241</v>
       </c>
     </row>
     <row r="29">
@@ -2499,16 +2499,16 @@
         <v>57</v>
       </c>
       <c r="B29" t="n">
-        <v>-319146.08488979</v>
+        <v>-453425.0593719763</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>106990.3675047242</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>-212155.7173850657</v>
+        <v>-453425.0593719763</v>
       </c>
     </row>
     <row r="30">
@@ -2516,16 +2516,16 @@
         <v>58</v>
       </c>
       <c r="B30" t="n">
-        <v>-282588.6868497225</v>
+        <v>-420035.8797422284</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>85682.18199699625</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>-196906.5048527262</v>
+        <v>-420035.8797422284</v>
       </c>
     </row>
     <row r="31">
@@ -2533,16 +2533,16 @@
         <v>59</v>
       </c>
       <c r="B31" t="n">
-        <v>-246031.2888096549</v>
+        <v>-386646.7001124805</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>66044.70196285787</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>-179986.586846797</v>
+        <v>-386646.7001124805</v>
       </c>
     </row>
     <row r="32">
@@ -2550,16 +2550,16 @@
         <v>60</v>
       </c>
       <c r="B32" t="n">
-        <v>-209473.8907695873</v>
+        <v>-353257.5204827326</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>48069.12732349004</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>-161404.7634460973</v>
+        <v>-353257.5204827326</v>
       </c>
     </row>
     <row r="33">
@@ -2567,16 +2567,16 @@
         <v>61</v>
       </c>
       <c r="B33" t="n">
-        <v>-172916.4927295198</v>
+        <v>-319868.3408529848</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>31725.40631977806</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>-141191.0864097417</v>
+        <v>-319868.3408529848</v>
       </c>
     </row>
     <row r="34">
@@ -2584,16 +2584,16 @@
         <v>62</v>
       </c>
       <c r="B34" t="n">
-        <v>-136359.0946894522</v>
+        <v>-286479.1612232369</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>16964.40005208955</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>-119394.6946373626</v>
+        <v>-286479.1612232369</v>
       </c>
     </row>
     <row r="35">
@@ -2601,16 +2601,16 @@
         <v>63</v>
       </c>
       <c r="B35" t="n">
-        <v>-99801.6966493846</v>
+        <v>-253089.9815934889</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>3720.556698971192</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>-96081.1399504134</v>
+        <v>-253089.9815934889</v>
       </c>
     </row>
     <row r="36">
@@ -2618,16 +2618,16 @@
         <v>64</v>
       </c>
       <c r="B36" t="n">
-        <v>-63244.29860931703</v>
+        <v>-219700.8019637411</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>-8085.096684545647</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>-71329.39529386268</v>
+        <v>-219700.8019637411</v>
       </c>
     </row>
     <row r="37">
@@ -2635,16 +2635,16 @@
         <v>65</v>
       </c>
       <c r="B37" t="n">
-        <v>-26686.90056924947</v>
+        <v>-186311.6223339932</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>-18541.82782527341</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>-45228.72839452288</v>
+        <v>-186311.6223339932</v>
       </c>
     </row>
     <row r="38">
@@ -2652,16 +2652,16 @@
         <v>66</v>
       </c>
       <c r="B38" t="n">
-        <v>9870.497470818098</v>
+        <v>-152922.4427042453</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>-27746.10096334487</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>-17875.60349252677</v>
+        <v>-152922.4427042453</v>
       </c>
     </row>
     <row r="39">
@@ -2669,16 +2669,16 @@
         <v>67</v>
       </c>
       <c r="B39" t="n">
-        <v>46427.89551088566</v>
+        <v>-119533.2630744974</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>-35798.64134349369</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>10629.25416739197</v>
+        <v>-119533.2630744974</v>
       </c>
     </row>
     <row r="40">
@@ -2686,16 +2686,16 @@
         <v>68</v>
       </c>
       <c r="B40" t="n">
-        <v>82985.29355095324</v>
+        <v>-86144.0834447495</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>-42801.76541008898</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>40183.52814086426</v>
+        <v>-86144.0834447495</v>
       </c>
     </row>
     <row r="41">
@@ -2703,16 +2703,16 @@
         <v>69</v>
       </c>
       <c r="B41" t="n">
-        <v>119542.6915910208</v>
+        <v>-52754.90381500161</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>-48857.047307464</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>70685.64428355679</v>
+        <v>-52754.90381500161</v>
       </c>
     </row>
     <row r="42">
@@ -2720,16 +2720,16 @@
         <v>70</v>
       </c>
       <c r="B42" t="n">
-        <v>156100.0896310884</v>
+        <v>-19365.72418525372</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>-54063.36187823371</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>102036.7277528547</v>
+        <v>-19365.72418525372</v>
       </c>
     </row>
     <row r="43">
@@ -2737,16 +2737,16 @@
         <v>71</v>
       </c>
       <c r="B43" t="n">
-        <v>192657.4876711559</v>
+        <v>14023.45544449417</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>-58515.31765809798</v>
+        <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>134142.1700130579</v>
+        <v>14023.45544449417</v>
       </c>
     </row>
     <row r="44">
@@ -2754,16 +2754,16 @@
         <v>72</v>
       </c>
       <c r="B44" t="n">
-        <v>229214.8857112235</v>
+        <v>47412.63507424206</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>-62302.07144038383</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>166912.8142708397</v>
+        <v>47412.63507424206</v>
       </c>
     </row>
     <row r="45">
@@ -2771,16 +2771,16 @@
         <v>73</v>
       </c>
       <c r="B45" t="n">
-        <v>265772.283751291</v>
+        <v>80801.81470398995</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>-65506.49924655697</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>200265.7845047341</v>
+        <v>80801.81470398995</v>
       </c>
     </row>
     <row r="46">
@@ -2788,16 +2788,16 @@
         <v>74</v>
       </c>
       <c r="B46" t="n">
-        <v>302329.6817913586</v>
+        <v>114190.9943337378</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>-68204.6869035831</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>234124.9948877755</v>
+        <v>114190.9943337378</v>
       </c>
     </row>
     <row r="47">
@@ -2805,16 +2805,16 @@
         <v>75</v>
       </c>
       <c r="B47" t="n">
-        <v>338887.0798314262</v>
+        <v>147580.1739634857</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>-70465.69644493578</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>268421.3833864904</v>
+        <v>147580.1739634857</v>
       </c>
     </row>
     <row r="48">
@@ -2822,16 +2822,16 @@
         <v>76</v>
       </c>
       <c r="B48" t="n">
-        <v>375444.4778714938</v>
+        <v>180969.3535932336</v>
       </c>
       <c r="C48" t="n">
         <v>0</v>
       </c>
       <c r="D48" t="n">
-        <v>-72351.56154054662</v>
+        <v>0</v>
       </c>
       <c r="E48" t="n">
-        <v>303092.9163309472</v>
+        <v>180969.3535932336</v>
       </c>
     </row>
     <row r="49">
@@ -2839,16 +2839,16 @@
         <v>77</v>
       </c>
       <c r="B49" t="n">
-        <v>412001.8759115613</v>
+        <v>214358.5332229815</v>
       </c>
       <c r="C49" t="n">
         <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>-73917.46533335123</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>338084.4105782101</v>
+        <v>214358.5332229815</v>
       </c>
     </row>
     <row r="50">
@@ -2856,16 +2856,16 @@
         <v>78</v>
       </c>
       <c r="B50" t="n">
-        <v>448559.2739516289</v>
+        <v>247747.7128527294</v>
       </c>
       <c r="C50" t="n">
         <v>0</v>
       </c>
       <c r="D50" t="n">
-        <v>-75212.05661070411</v>
+        <v>0</v>
       </c>
       <c r="E50" t="n">
-        <v>373347.2173409248</v>
+        <v>247747.7128527294</v>
       </c>
     </row>
     <row r="51">
@@ -2873,16 +2873,16 @@
         <v>79</v>
       </c>
       <c r="B51" t="n">
-        <v>485116.6719916964</v>
+        <v>281136.8924824773</v>
       </c>
       <c r="C51" t="n">
         <v>0</v>
       </c>
       <c r="D51" t="n">
-        <v>-76277.86441333281</v>
+        <v>0</v>
       </c>
       <c r="E51" t="n">
-        <v>408838.8075783636</v>
+        <v>281136.8924824773</v>
       </c>
     </row>
     <row r="52">
@@ -2890,16 +2890,16 @@
         <v>80</v>
       </c>
       <c r="B52" t="n">
-        <v>521674.070031764</v>
+        <v>314526.0721122252</v>
       </c>
       <c r="C52" t="n">
         <v>0</v>
       </c>
       <c r="D52" t="n">
-        <v>-77151.77632234343</v>
+        <v>0</v>
       </c>
       <c r="E52" t="n">
-        <v>444522.2937094206</v>
+        <v>314526.0721122252</v>
       </c>
     </row>
     <row r="53">
@@ -2907,16 +2907,16 @@
         <v>81</v>
       </c>
       <c r="B53" t="n">
-        <v>558231.4680718316</v>
+        <v>347915.2517419731</v>
       </c>
       <c r="C53" t="n">
         <v>0</v>
       </c>
       <c r="D53" t="n">
-        <v>-77865.55122238146</v>
+        <v>0</v>
       </c>
       <c r="E53" t="n">
-        <v>480365.9168494502</v>
+        <v>347915.2517419731</v>
       </c>
     </row>
     <row r="54">
@@ -2924,16 +2924,16 @@
         <v>82</v>
       </c>
       <c r="B54" t="n">
-        <v>594788.8661118991</v>
+        <v>381304.431371721</v>
       </c>
       <c r="C54" t="n">
         <v>0</v>
       </c>
       <c r="D54" t="n">
-        <v>-78446.34289555173</v>
+        <v>0</v>
       </c>
       <c r="E54" t="n">
-        <v>516342.5232163474</v>
+        <v>381304.431371721</v>
       </c>
     </row>
     <row r="55">
@@ -2941,16 +2941,16 @@
         <v>83</v>
       </c>
       <c r="B55" t="n">
-        <v>631346.2641519668</v>
+        <v>414693.6110014688</v>
       </c>
       <c r="C55" t="n">
         <v>0</v>
       </c>
       <c r="D55" t="n">
-        <v>-78917.21605238349</v>
+        <v>0</v>
       </c>
       <c r="E55" t="n">
-        <v>552429.0480995832</v>
+        <v>414693.6110014688</v>
       </c>
     </row>
     <row r="56">
@@ -2958,16 +2958,16 @@
         <v>84</v>
       </c>
       <c r="B56" t="n">
-        <v>667903.6621920343</v>
+        <v>448082.7906312168</v>
       </c>
       <c r="C56" t="n">
         <v>0</v>
       </c>
       <c r="D56" t="n">
-        <v>-79297.64115342071</v>
+        <v>0</v>
       </c>
       <c r="E56" t="n">
-        <v>588606.0210386136</v>
+        <v>448082.7906312168</v>
       </c>
     </row>
     <row r="57">
@@ -2975,16 +2975,16 @@
         <v>85</v>
       </c>
       <c r="B57" t="n">
-        <v>704461.0602321018</v>
+        <v>481471.9702609646</v>
       </c>
       <c r="C57" t="n">
         <v>0</v>
       </c>
       <c r="D57" t="n">
-        <v>-79603.95850536569</v>
+        <v>0</v>
       </c>
       <c r="E57" t="n">
-        <v>624857.1017267362</v>
+        <v>481471.9702609646</v>
       </c>
     </row>
     <row r="58">
@@ -2992,16 +2992,16 @@
         <v>86</v>
       </c>
       <c r="B58" t="n">
-        <v>741018.4582721695</v>
+        <v>514861.1498907126</v>
       </c>
       <c r="C58" t="n">
         <v>0</v>
       </c>
       <c r="D58" t="n">
-        <v>-79849.80558524202</v>
+        <v>0</v>
       </c>
       <c r="E58" t="n">
-        <v>661168.6526869275</v>
+        <v>514861.1498907126</v>
       </c>
     </row>
     <row r="59">
@@ -3009,16 +3009,16 @@
         <v>87</v>
       </c>
       <c r="B59" t="n">
-        <v>777575.856312237</v>
+        <v>548250.3295204605</v>
       </c>
       <c r="C59" t="n">
         <v>0</v>
       </c>
       <c r="D59" t="n">
-        <v>-80046.50436190891</v>
+        <v>0</v>
       </c>
       <c r="E59" t="n">
-        <v>697529.3519503281</v>
+        <v>548250.3295204605</v>
       </c>
     </row>
     <row r="60">
@@ -3026,16 +3026,16 @@
         <v>88</v>
       </c>
       <c r="B60" t="n">
-        <v>814133.2543523046</v>
+        <v>581639.5091502083</v>
       </c>
       <c r="C60" t="n">
         <v>0</v>
       </c>
       <c r="D60" t="n">
-        <v>-80203.40758873863</v>
+        <v>0</v>
       </c>
       <c r="E60" t="n">
-        <v>733929.846763566</v>
+        <v>581639.5091502083</v>
       </c>
     </row>
     <row r="61">
@@ -3043,16 +3043,16 @@
         <v>89</v>
       </c>
       <c r="B61" t="n">
-        <v>850690.6523923721</v>
+        <v>615028.6887799562</v>
       </c>
       <c r="C61" t="n">
         <v>0</v>
       </c>
       <c r="D61" t="n">
-        <v>-80328.20469846611</v>
+        <v>0</v>
       </c>
       <c r="E61" t="n">
-        <v>770362.447693906</v>
+        <v>615028.6887799562</v>
       </c>
     </row>
     <row r="62">
@@ -3060,16 +3060,16 @@
         <v>90</v>
       </c>
       <c r="B62" t="n">
-        <v>887248.0504324398</v>
+        <v>648417.8684097041</v>
       </c>
       <c r="C62" t="n">
         <v>0</v>
       </c>
       <c r="D62" t="n">
-        <v>-80427.18911640198</v>
+        <v>0</v>
       </c>
       <c r="E62" t="n">
-        <v>806820.8613160378</v>
+        <v>648417.8684097041</v>
       </c>
     </row>
     <row r="63">
@@ -3077,16 +3077,16 @@
         <v>91</v>
       </c>
       <c r="B63" t="n">
-        <v>923805.4484725072</v>
+        <v>681807.0480394519</v>
       </c>
       <c r="C63" t="n">
         <v>0</v>
       </c>
       <c r="D63" t="n">
-        <v>-80505.4895998041</v>
+        <v>0</v>
       </c>
       <c r="E63" t="n">
-        <v>843299.9588727031</v>
+        <v>681807.0480394519</v>
       </c>
     </row>
     <row r="64">
@@ -3094,16 +3094,16 @@
         <v>92</v>
       </c>
       <c r="B64" t="n">
-        <v>960362.8465125748</v>
+        <v>715196.2276691998</v>
       </c>
       <c r="C64" t="n">
         <v>0</v>
       </c>
       <c r="D64" t="n">
-        <v>-80567.26868514891</v>
+        <v>0</v>
       </c>
       <c r="E64" t="n">
-        <v>879795.5778274259</v>
+        <v>715196.2276691998</v>
       </c>
     </row>
     <row r="65">
@@ -3111,16 +3111,16 @@
         <v>93</v>
       </c>
       <c r="B65" t="n">
-        <v>996920.2445526423</v>
+        <v>748585.4072989478</v>
       </c>
       <c r="C65" t="n">
         <v>0</v>
       </c>
       <c r="D65" t="n">
-        <v>-80615.89155107201</v>
+        <v>0</v>
       </c>
       <c r="E65" t="n">
-        <v>916304.3530015703</v>
+        <v>748585.4072989478</v>
       </c>
     </row>
     <row r="66">
@@ -3128,16 +3128,16 @@
         <v>94</v>
       </c>
       <c r="B66" t="n">
-        <v>1033477.64259271</v>
+        <v>781974.5869286957</v>
       </c>
       <c r="C66" t="n">
         <v>0</v>
       </c>
       <c r="D66" t="n">
-        <v>-80654.06864430483</v>
+        <v>0</v>
       </c>
       <c r="E66" t="n">
-        <v>952823.5739484051</v>
+        <v>781974.5869286957</v>
       </c>
     </row>
     <row r="67">
@@ -3145,16 +3145,16 @@
         <v>95</v>
       </c>
       <c r="B67" t="n">
-        <v>1070035.040632778</v>
+        <v>815363.7665584435</v>
       </c>
       <c r="C67" t="n">
         <v>0</v>
       </c>
       <c r="D67" t="n">
-        <v>-80683.97532129315</v>
+        <v>0</v>
       </c>
       <c r="E67" t="n">
-        <v>989351.0653114845</v>
+        <v>815363.7665584435</v>
       </c>
     </row>
     <row r="68">
@@ -3162,16 +3162,16 @@
         <v>96</v>
       </c>
       <c r="B68" t="n">
-        <v>1106592.438672845</v>
+        <v>848752.9461881914</v>
       </c>
       <c r="C68" t="n">
         <v>0</v>
       </c>
       <c r="D68" t="n">
-        <v>-80707.35157240221</v>
+        <v>0</v>
       </c>
       <c r="E68" t="n">
-        <v>1025885.087100443</v>
+        <v>848752.9461881914</v>
       </c>
     </row>
     <row r="69">
@@ -3179,16 +3179,16 @@
         <v>97</v>
       </c>
       <c r="B69" t="n">
-        <v>1143149.836712913</v>
+        <v>882142.1258179394</v>
       </c>
       <c r="C69" t="n">
         <v>0</v>
       </c>
       <c r="D69" t="n">
-        <v>-80725.58465308472</v>
+        <v>0</v>
       </c>
       <c r="E69" t="n">
-        <v>1062424.252059828</v>
+        <v>882142.1258179394</v>
       </c>
     </row>
     <row r="70">
@@ -3196,16 +3196,16 @@
         <v>98</v>
       </c>
       <c r="B70" t="n">
-        <v>1179707.23475298</v>
+        <v>915531.3054476872</v>
       </c>
       <c r="C70" t="n">
         <v>0</v>
       </c>
       <c r="D70" t="n">
-        <v>-80739.77717371962</v>
+        <v>0</v>
       </c>
       <c r="E70" t="n">
-        <v>1098967.457579261</v>
+        <v>915531.3054476872</v>
       </c>
     </row>
     <row r="71">
@@ -3213,16 +3213,16 @@
         <v>99</v>
       </c>
       <c r="B71" t="n">
-        <v>1216264.632793048</v>
+        <v>948920.485077435</v>
       </c>
       <c r="C71" t="n">
         <v>0</v>
       </c>
       <c r="D71" t="n">
-        <v>-80750.80291690626</v>
+        <v>0</v>
       </c>
       <c r="E71" t="n">
-        <v>1135513.829876141</v>
+        <v>948920.485077435</v>
       </c>
     </row>
     <row r="72">
@@ -3230,16 +3230,16 @@
         <v>100</v>
       </c>
       <c r="B72" t="n">
-        <v>1252822.030833115</v>
+        <v>982309.664707183</v>
       </c>
       <c r="C72" t="n">
         <v>0</v>
       </c>
       <c r="D72" t="n">
-        <v>-80759.35237208089</v>
+        <v>0</v>
       </c>
       <c r="E72" t="n">
-        <v>1172062.678461035</v>
+        <v>982309.664707183</v>
       </c>
     </row>
   </sheetData>
@@ -3293,16 +3293,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="n">
-        <v>-914858.7112627907</v>
+        <v>-838957.4106661081</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>463644.3259996536</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>-451214.3852631371</v>
+        <v>-838957.4106661081</v>
       </c>
     </row>
     <row r="3">
@@ -3310,16 +3310,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="n">
-        <v>-855336.3487863566</v>
+        <v>-778251.3751620481</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>410373.6864873929</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
-        <v>-444962.6622989637</v>
+        <v>-778251.3751620481</v>
       </c>
     </row>
     <row r="4">
@@ -3327,16 +3327,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>-795813.9863099226</v>
+        <v>-717545.3396579883</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>359240.1255128458</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>-436573.8607970768</v>
+        <v>-717545.3396579883</v>
       </c>
     </row>
     <row r="5">
@@ -3344,16 +3344,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>-736291.6238334887</v>
+        <v>-656839.3041539284</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>310615.6233353584</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>-425676.0004981303</v>
+        <v>-656839.3041539284</v>
       </c>
     </row>
     <row r="6">
@@ -3361,16 +3361,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>-676769.2613570547</v>
+        <v>-596133.2686498684</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>264831.3926175556</v>
+        <v>0</v>
       </c>
       <c r="E6" t="n">
-        <v>-411937.8687394991</v>
+        <v>-596133.2686498684</v>
       </c>
     </row>
     <row r="7">
@@ -3378,16 +3378,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>-617246.8988806206</v>
+        <v>-535427.2331458085</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>222158.3159678898</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>-395088.5829127308</v>
+        <v>-535427.2331458085</v>
       </c>
     </row>
     <row r="8">
@@ -3395,16 +3395,16 @@
         <v>31</v>
       </c>
       <c r="B8" t="n">
-        <v>-557724.5364041866</v>
+        <v>-474721.1976417486</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>182793.2333709712</v>
+        <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>-374931.3030332155</v>
+        <v>-474721.1976417486</v>
       </c>
     </row>
     <row r="9">
@@ -3412,16 +3412,16 @@
         <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>-498202.1739277526</v>
+        <v>-414015.1621376887</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>146851.8825032357</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>-351350.2914245169</v>
+        <v>-414015.1621376887</v>
       </c>
     </row>
     <row r="10">
@@ -3429,16 +3429,16 @@
         <v>33</v>
       </c>
       <c r="B10" t="n">
-        <v>-438679.8114513186</v>
+        <v>-353309.1266336287</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>114368.3351357345</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>-324311.476315584</v>
+        <v>-353309.1266336287</v>
       </c>
     </row>
     <row r="11">
@@ -3446,16 +3446,16 @@
         <v>34</v>
       </c>
       <c r="B11" t="n">
-        <v>-379157.4489748845</v>
+        <v>-292603.0911295689</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>85300.03572669653</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
-        <v>-293857.413248188</v>
+        <v>-292603.0911295689</v>
       </c>
     </row>
     <row r="12">
@@ -3463,16 +3463,16 @@
         <v>35</v>
       </c>
       <c r="B12" t="n">
-        <v>-319635.0864984505</v>
+        <v>-231897.0556255089</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>59537.09720702739</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>-260097.9892914232</v>
+        <v>-231897.0556255089</v>
       </c>
     </row>
     <row r="13">
@@ -3480,16 +3480,16 @@
         <v>36</v>
       </c>
       <c r="B13" t="n">
-        <v>-260112.7240220165</v>
+        <v>-171191.020121449</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>36914.3374782612</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
-        <v>-223198.3865437553</v>
+        <v>-171191.020121449</v>
       </c>
     </row>
     <row r="14">
@@ -3497,16 +3497,16 @@
         <v>37</v>
       </c>
       <c r="B14" t="n">
-        <v>-200590.3615455825</v>
+        <v>-110484.9846173891</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>17224.59640457542</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
-        <v>-183365.7651410071</v>
+        <v>-110484.9846173891</v>
       </c>
     </row>
     <row r="15">
@@ -3514,16 +3514,16 @@
         <v>38</v>
       </c>
       <c r="B15" t="n">
-        <v>-141067.9990691485</v>
+        <v>-49778.94911332915</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>232.0846602225455</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>-140835.9144089259</v>
+        <v>-49778.94911332915</v>
       </c>
     </row>
     <row r="16">
@@ -3531,16 +3531,16 @@
         <v>39</v>
       </c>
       <c r="B16" t="n">
-        <v>-81545.63659271445</v>
+        <v>10927.08639073077</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-14315.19048918657</v>
+        <v>0</v>
       </c>
       <c r="E16" t="n">
-        <v>-95860.82708190102</v>
+        <v>10927.08639073077</v>
       </c>
     </row>
     <row r="17">
@@ -3548,16 +3548,16 @@
         <v>40</v>
       </c>
       <c r="B17" t="n">
-        <v>-22023.27411628044</v>
+        <v>71633.12189479069</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-26674.56295064781</v>
+        <v>0</v>
       </c>
       <c r="E17" t="n">
-        <v>-48697.83706692825</v>
+        <v>71633.12189479069</v>
       </c>
     </row>
     <row r="18">
@@ -3565,16 +3565,16 @@
         <v>41</v>
       </c>
       <c r="B18" t="n">
-        <v>37499.08836015358</v>
+        <v>132339.1573988506</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-37099.75843130075</v>
+        <v>0</v>
       </c>
       <c r="E18" t="n">
-        <v>399.329928852836</v>
+        <v>132339.1573988506</v>
       </c>
     </row>
     <row r="19">
@@ -3582,16 +3582,16 @@
         <v>42</v>
       </c>
       <c r="B19" t="n">
-        <v>97021.4508365876</v>
+        <v>193045.1929029105</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-45833.96550728285</v>
+        <v>0</v>
       </c>
       <c r="E19" t="n">
-        <v>51187.48532930474</v>
+        <v>193045.1929029105</v>
       </c>
     </row>
     <row r="20">
@@ -3599,16 +3599,16 @@
         <v>43</v>
       </c>
       <c r="B20" t="n">
-        <v>156543.8133130216</v>
+        <v>253751.2284069704</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-53104.85333491098</v>
+        <v>0</v>
       </c>
       <c r="E20" t="n">
-        <v>103438.9599781106</v>
+        <v>253751.2284069704</v>
       </c>
     </row>
     <row r="21">
@@ -3616,16 +3616,16 @@
         <v>44</v>
       </c>
       <c r="B21" t="n">
-        <v>216066.1757894557</v>
+        <v>314457.2639110303</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-59121.34098265524</v>
+        <v>0</v>
       </c>
       <c r="E21" t="n">
-        <v>156944.8348068004</v>
+        <v>314457.2639110303</v>
       </c>
     </row>
     <row r="22">
@@ -3633,16 +3633,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="n">
-        <v>275588.5382658896</v>
+        <v>375163.2994150903</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-64071.85508446302</v>
+        <v>0</v>
       </c>
       <c r="E22" t="n">
-        <v>211516.6831814266</v>
+        <v>375163.2994150903</v>
       </c>
     </row>
     <row r="23">
@@ -3650,16 +3650,16 @@
         <v>46</v>
       </c>
       <c r="B23" t="n">
-        <v>335110.9007423237</v>
+        <v>435869.3349191502</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-68123.78651100947</v>
+        <v>0</v>
       </c>
       <c r="E23" t="n">
-        <v>266987.1142313142</v>
+        <v>435869.3349191502</v>
       </c>
     </row>
     <row r="24">
@@ -3667,16 +3667,16 @@
         <v>47</v>
       </c>
       <c r="B24" t="n">
-        <v>394633.2632187577</v>
+        <v>496575.3704232101</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-71423.86151720458</v>
+        <v>0</v>
       </c>
       <c r="E24" t="n">
-        <v>323209.4017015531</v>
+        <v>496575.3704232101</v>
       </c>
     </row>
     <row r="25">
@@ -3684,16 +3684,16 @@
         <v>48</v>
       </c>
       <c r="B25" t="n">
-        <v>454155.6256951917</v>
+        <v>557281.4059272701</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-74099.16770019024</v>
+        <v>0</v>
       </c>
       <c r="E25" t="n">
-        <v>380056.4579950015</v>
+        <v>557281.4059272701</v>
       </c>
     </row>
     <row r="26">
@@ -3701,16 +3701,16 @@
         <v>49</v>
       </c>
       <c r="B26" t="n">
-        <v>513677.9881716256</v>
+        <v>617987.4414313299</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-76258.61120402</v>
+        <v>0</v>
       </c>
       <c r="E26" t="n">
-        <v>437419.3769676057</v>
+        <v>617987.4414313299</v>
       </c>
     </row>
     <row r="27">
@@ -3718,16 +3718,16 @@
         <v>50</v>
       </c>
       <c r="B27" t="n">
-        <v>573200.3506480597</v>
+        <v>678693.4769353899</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-77994.62213326278</v>
+        <v>0</v>
       </c>
       <c r="E27" t="n">
-        <v>495205.7285147969</v>
+        <v>678693.4769353899</v>
       </c>
     </row>
     <row r="28">
@@ -3735,16 +3735,16 @@
         <v>51</v>
       </c>
       <c r="B28" t="n">
-        <v>632722.7131244937</v>
+        <v>739399.5124394498</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-79384.96531188441</v>
+        <v>0</v>
       </c>
       <c r="E28" t="n">
-        <v>553337.7478126093</v>
+        <v>739399.5124394498</v>
       </c>
     </row>
     <row r="29">
@@ -3752,16 +3752,16 @@
         <v>52</v>
       </c>
       <c r="B29" t="n">
-        <v>692245.0756009278</v>
+        <v>800105.5479435096</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-80494.5503218165</v>
+        <v>0</v>
       </c>
       <c r="E29" t="n">
-        <v>611750.5252791113</v>
+        <v>800105.5479435096</v>
       </c>
     </row>
     <row r="30">
@@ -3769,16 +3769,16 @@
         <v>53</v>
       </c>
       <c r="B30" t="n">
-        <v>751767.4380773618</v>
+        <v>860811.5834475696</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-81377.16654213429</v>
+        <v>0</v>
       </c>
       <c r="E30" t="n">
-        <v>670390.2715352275</v>
+        <v>860811.5834475696</v>
       </c>
     </row>
     <row r="31">
@@ -3786,16 +3786,16 @@
         <v>54</v>
       </c>
       <c r="B31" t="n">
-        <v>811289.8005537959</v>
+        <v>921517.6189516296</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-82077.09506748866</v>
+        <v>0</v>
       </c>
       <c r="E31" t="n">
-        <v>729212.7054863073</v>
+        <v>921517.6189516296</v>
       </c>
     </row>
     <row r="32">
@@ -3803,16 +3803,16 @@
         <v>55</v>
       </c>
       <c r="B32" t="n">
-        <v>870812.1630302299</v>
+        <v>982223.6544556894</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-82630.56998401765</v>
+        <v>0</v>
       </c>
       <c r="E32" t="n">
-        <v>788181.5930462122</v>
+        <v>982223.6544556894</v>
       </c>
     </row>
     <row r="33">
@@ -3820,16 +3820,16 @@
         <v>56</v>
       </c>
       <c r="B33" t="n">
-        <v>930334.5255066638</v>
+        <v>1042929.689959749</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>-83067.07701189739</v>
+        <v>0</v>
       </c>
       <c r="E33" t="n">
-        <v>847267.4484947665</v>
+        <v>1042929.689959749</v>
       </c>
     </row>
     <row r="34">
@@ -3837,16 +3837,16 @@
         <v>57</v>
       </c>
       <c r="B34" t="n">
-        <v>989856.8879830979</v>
+        <v>1103635.725463809</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>-83410.4886910362</v>
+        <v>0</v>
       </c>
       <c r="E34" t="n">
-        <v>906446.3992920617</v>
+        <v>1103635.725463809</v>
       </c>
     </row>
     <row r="35">
@@ -3854,16 +3854,16 @@
         <v>58</v>
       </c>
       <c r="B35" t="n">
-        <v>1049379.250459532</v>
+        <v>1164341.760967869</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>-83680.04286788909</v>
+        <v>0</v>
       </c>
       <c r="E35" t="n">
-        <v>965699.207591643</v>
+        <v>1164341.760967869</v>
       </c>
     </row>
     <row r="36">
@@ -3871,16 +3871,16 @@
         <v>59</v>
       </c>
       <c r="B36" t="n">
-        <v>1108901.612935966</v>
+        <v>1225047.796471929</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>-83891.17599461526</v>
+        <v>0</v>
       </c>
       <c r="E36" t="n">
-        <v>1025010.436941351</v>
+        <v>1225047.796471929</v>
       </c>
     </row>
     <row r="37">
@@ -3888,16 +3888,16 @@
         <v>60</v>
       </c>
       <c r="B37" t="n">
-        <v>1168423.9754124</v>
+        <v>1285753.831975989</v>
       </c>
       <c r="C37" t="n">
         <v>0</v>
       </c>
       <c r="D37" t="n">
-        <v>-84056.22536052484</v>
+        <v>0</v>
       </c>
       <c r="E37" t="n">
-        <v>1084367.750051875</v>
+        <v>1285753.831975989</v>
       </c>
     </row>
     <row r="38">
@@ -3905,16 +3905,16 @@
         <v>61</v>
       </c>
       <c r="B38" t="n">
-        <v>1227946.337888834</v>
+        <v>1346459.867480049</v>
       </c>
       <c r="C38" t="n">
         <v>0</v>
       </c>
       <c r="D38" t="n">
-        <v>-84185.01542386513</v>
+        <v>0</v>
       </c>
       <c r="E38" t="n">
-        <v>1143761.322464969</v>
+        <v>1346459.867480049</v>
       </c>
     </row>
     <row r="39">
@@ -3922,16 +3922,16 @@
         <v>62</v>
       </c>
       <c r="B39" t="n">
-        <v>1287468.700365268</v>
+        <v>1407165.902984109</v>
       </c>
       <c r="C39" t="n">
         <v>0</v>
       </c>
       <c r="D39" t="n">
-        <v>-84285.34337666682</v>
+        <v>0</v>
       </c>
       <c r="E39" t="n">
-        <v>1203183.356988601</v>
+        <v>1407165.902984109</v>
       </c>
     </row>
     <row r="40">
@@ -3939,16 +3939,16 @@
         <v>63</v>
       </c>
       <c r="B40" t="n">
-        <v>1346991.062841702</v>
+        <v>1467871.938488169</v>
       </c>
       <c r="C40" t="n">
         <v>0</v>
       </c>
       <c r="D40" t="n">
-        <v>-84363.37833188973</v>
+        <v>0</v>
       </c>
       <c r="E40" t="n">
-        <v>1262627.684509812</v>
+        <v>1467871.938488169</v>
       </c>
     </row>
     <row r="41">
@@ -3956,16 +3956,16 @@
         <v>64</v>
       </c>
       <c r="B41" t="n">
-        <v>1406513.425318136</v>
+        <v>1528577.973992229</v>
       </c>
       <c r="C41" t="n">
         <v>0</v>
       </c>
       <c r="D41" t="n">
-        <v>-84423.98735514756</v>
+        <v>0</v>
       </c>
       <c r="E41" t="n">
-        <v>1322089.437962988</v>
+        <v>1528577.973992229</v>
       </c>
     </row>
     <row r="42">
@@ -3973,16 +3973,16 @@
         <v>65</v>
       </c>
       <c r="B42" t="n">
-        <v>1466035.78779457</v>
+        <v>1589284.009496289</v>
       </c>
       <c r="C42" t="n">
         <v>0</v>
       </c>
       <c r="D42" t="n">
-        <v>-84471.00018098264</v>
+        <v>0</v>
       </c>
       <c r="E42" t="n">
-        <v>1381564.787613587</v>
+        <v>1589284.009496289</v>
       </c>
     </row>
     <row r="43">
@@ -3990,16 +3990,16 @@
         <v>66</v>
       </c>
       <c r="B43" t="n">
-        <v>1525558.150271004</v>
+        <v>1649990.045000348</v>
       </c>
       <c r="C43" t="n">
         <v>0</v>
       </c>
       <c r="D43" t="n">
-        <v>-84507.42300210184</v>
+        <v>0</v>
       </c>
       <c r="E43" t="n">
-        <v>1441050.727268902</v>
+        <v>1649990.045000348</v>
       </c>
     </row>
     <row r="44">
@@ -4007,16 +4007,16 @@
         <v>67</v>
       </c>
       <c r="B44" t="n">
-        <v>1585080.512747438</v>
+        <v>1710696.080504408</v>
       </c>
       <c r="C44" t="n">
         <v>0</v>
       </c>
       <c r="D44" t="n">
-        <v>-84535.61029674204</v>
+        <v>0</v>
       </c>
       <c r="E44" t="n">
-        <v>1500544.902450696</v>
+        <v>1710696.080504408</v>
       </c>
     </row>
     <row r="45">
@@ -4024,16 +4024,16 @@
         <v>68</v>
       </c>
       <c r="B45" t="n">
-        <v>1644602.875223872</v>
+        <v>1771402.116008468</v>
       </c>
       <c r="C45" t="n">
         <v>0</v>
       </c>
       <c r="D45" t="n">
-        <v>-84557.40232528433</v>
+        <v>0</v>
       </c>
       <c r="E45" t="n">
-        <v>1560045.472898588</v>
+        <v>1771402.116008468</v>
       </c>
     </row>
     <row r="46">
@@ -4041,16 +4041,16 @@
         <v>69</v>
       </c>
       <c r="B46" t="n">
-        <v>1704125.237700306</v>
+        <v>1832108.151512528</v>
       </c>
       <c r="C46" t="n">
         <v>0</v>
       </c>
       <c r="D46" t="n">
-        <v>-84574.23471639969</v>
+        <v>0</v>
       </c>
       <c r="E46" t="n">
-        <v>1619551.002983906</v>
+        <v>1832108.151512528</v>
       </c>
     </row>
     <row r="47">
@@ -4058,16 +4058,16 @@
         <v>70</v>
       </c>
       <c r="B47" t="n">
-        <v>1763647.60017674</v>
+        <v>1892814.187016588</v>
       </c>
       <c r="C47" t="n">
         <v>0</v>
       </c>
       <c r="D47" t="n">
-        <v>-84587.2254904712</v>
+        <v>0</v>
       </c>
       <c r="E47" t="n">
-        <v>1679060.374686269</v>
+        <v>1892814.187016588</v>
       </c>
     </row>
   </sheetData>
@@ -4121,16 +4121,16 @@
         <v>25</v>
       </c>
       <c r="B2" t="n">
-        <v>-671196.6210704048</v>
+        <v>-637370.3534764132</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
       </c>
       <c r="D2" t="n">
-        <v>446327.987600325</v>
+        <v>349806.1717820855</v>
       </c>
       <c r="E2" t="n">
-        <v>-224868.6334700798</v>
+        <v>-287564.1816943277</v>
       </c>
     </row>
     <row r="3">
@@ -4138,16 +4138,16 @@
         <v>26</v>
       </c>
       <c r="B3" t="n">
-        <v>-602143.4707545195</v>
+        <v>-569129.4162733712</v>
       </c>
       <c r="C3" t="n">
         <v>0</v>
       </c>
       <c r="D3" t="n">
-        <v>380732.4634014136</v>
+        <v>296240.6332573061</v>
       </c>
       <c r="E3" t="n">
-        <v>-221411.0073531058</v>
+        <v>-272888.7830160651</v>
       </c>
     </row>
     <row r="4">
@@ -4155,16 +4155,16 @@
         <v>27</v>
       </c>
       <c r="B4" t="n">
-        <v>-533090.3204386343</v>
+        <v>-500888.4790703291</v>
       </c>
       <c r="C4" t="n">
         <v>0</v>
       </c>
       <c r="D4" t="n">
-        <v>317185.787562877</v>
+        <v>245778.2947253204</v>
       </c>
       <c r="E4" t="n">
-        <v>-215904.5328757573</v>
+        <v>-255110.1843450087</v>
       </c>
     </row>
     <row r="5">
@@ -4172,16 +4172,16 @@
         <v>28</v>
       </c>
       <c r="B5" t="n">
-        <v>-464037.1701227489</v>
+        <v>-432647.541867287</v>
       </c>
       <c r="C5" t="n">
         <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>256475.7690841295</v>
+        <v>198625.5893651704</v>
       </c>
       <c r="E5" t="n">
-        <v>-207561.4010386195</v>
+        <v>-234021.9525021166</v>
       </c>
     </row>
     <row r="6">
@@ -4189,16 +4189,16 @@
         <v>29</v>
       </c>
       <c r="B6" t="n">
-        <v>-394984.0198068637</v>
+        <v>-364406.6046642449</v>
       </c>
       <c r="C6" t="n">
         <v>0</v>
       </c>
       <c r="D6" t="n">
-        <v>199422.7386651576</v>
+        <v>154919.6468444581</v>
       </c>
       <c r="E6" t="n">
-        <v>-195561.2811417061</v>
+        <v>-209486.9578197869</v>
       </c>
     </row>
     <row r="7">
@@ -4206,16 +4206,16 @@
         <v>30</v>
       </c>
       <c r="B7" t="n">
-        <v>-325930.8694909784</v>
+        <v>-296165.6674612028</v>
       </c>
       <c r="C7" t="n">
         <v>0</v>
       </c>
       <c r="D7" t="n">
-        <v>146790.0869911512</v>
+        <v>114727.242008901</v>
       </c>
       <c r="E7" t="n">
-        <v>-179140.7824998272</v>
+        <v>-181438.4254523019</v>
       </c>
     </row>
     <row r="8">
@@ -4223,16 +4223,16 @@
         <v>31</v>
       </c>
       <c r="B8" t="n">
-        <v>-256877.7191750931</v>
+        <v>-227924.7302581607</v>
       </c>
       <c r="C8" t="n">
         <v>0</v>
       </c>
       <c r="D8" t="n">
-        <v>99197.81685373558</v>
+        <v>78047.9652999643</v>
       </c>
       <c r="E8" t="n">
-        <v>-157679.9023213575</v>
+        <v>-149876.7649581964</v>
       </c>
     </row>
     <row r="9">
@@ -4240,16 +4240,16 @@
         <v>32</v>
       </c>
       <c r="B9" t="n">
-        <v>-187824.5688592079</v>
+        <v>-159683.7930551187</v>
       </c>
       <c r="C9" t="n">
         <v>0</v>
       </c>
       <c r="D9" t="n">
-        <v>57056.62216575383</v>
+        <v>44820.65469030914</v>
       </c>
       <c r="E9" t="n">
-        <v>-130767.946693454</v>
+        <v>-114863.1383648096</v>
       </c>
     </row>
     <row r="10">
@@ -4257,16 +4257,16 @@
         <v>33</v>
       </c>
       <c r="B10" t="n">
-        <v>-118771.4185433226</v>
+        <v>-91442.85585207661</v>
       </c>
       <c r="C10" t="n">
         <v>0</v>
       </c>
       <c r="D10" t="n">
-        <v>20533.68941612465</v>
+        <v>14932.04022333909</v>
       </c>
       <c r="E10" t="n">
-        <v>-98237.72912719793</v>
+        <v>-76510.81562873752</v>
       </c>
     </row>
     <row r="11">
@@ -4274,16 +4274,16 @@
         <v>34</v>
       </c>
       <c r="B11" t="n">
-        <v>-49718.26822743731</v>
+        <v>-23201.91864903453</v>
       </c>
       <c r="C11" t="n">
         <v>0</v>
       </c>
       <c r="D11" t="n">
-        <v>-10447.03457042626</v>
+        <v>-11773.4019804814</v>
       </c>
       <c r="E11" t="n">
-        <v>-60165.30279786357</v>
+        <v>-34975.32062951594</v>
       </c>
     </row>
     <row r="12">
@@ -4291,16 +4291,16 @@
         <v>35</v>
       </c>
       <c r="B12" t="n">
-        <v>19334.88208844795</v>
+        <v>45039.01855400753</v>
       </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>-36174.99048275029</v>
+        <v>-35483.25476017226</v>
       </c>
       <c r="E12" t="n">
-        <v>-16840.10839430234</v>
+        <v>9555.763793835271</v>
       </c>
     </row>
     <row r="13">
@@ -4308,16 +4308,16 @@
         <v>36</v>
       </c>
       <c r="B13" t="n">
-        <v>88388.03240433322</v>
+        <v>113279.9557570496</v>
       </c>
       <c r="C13" t="n">
         <v>0</v>
       </c>
       <c r="D13" t="n">
-        <v>-57103.29724376569</v>
+        <v>-56407.31134536836</v>
       </c>
       <c r="E13" t="n">
-        <v>31284.73516056754</v>
+        <v>56872.64441168123</v>
       </c>
     </row>
     <row r="14">
@@ -4325,16 +4325,16 @@
         <v>37</v>
       </c>
       <c r="B14" t="n">
-        <v>157441.1827202185</v>
+        <v>181520.8929600917</v>
       </c>
       <c r="C14" t="n">
         <v>0</v>
       </c>
       <c r="D14" t="n">
-        <v>-73790.41605585119</v>
+        <v>-74768.56684080086</v>
       </c>
       <c r="E14" t="n">
-        <v>83650.7666643673</v>
+        <v>106752.3261192908</v>
       </c>
     </row>
     <row r="15">
@@ -4342,16 +4342,16 @@
         <v>38</v>
       </c>
       <c r="B15" t="n">
-        <v>226494.3330361038</v>
+        <v>249761.8301631338</v>
       </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>-86843.15186118422</v>
+        <v>-90795.36116821243</v>
       </c>
       <c r="E15" t="n">
-        <v>139651.1811749195</v>
+        <v>158966.4689949213</v>
       </c>
     </row>
     <row r="16">
@@ -4359,16 +4359,16 @@
         <v>39</v>
       </c>
       <c r="B16" t="n">
-        <v>295547.483351989</v>
+        <v>318002.7673661758</v>
       </c>
       <c r="C16" t="n">
         <v>0</v>
       </c>
       <c r="D16" t="n">
-        <v>-96868.06398252149</v>
+        <v>-104714.8285090006</v>
       </c>
       <c r="E16" t="n">
-        <v>198679.4193694675</v>
+        <v>213287.9388571752</v>
       </c>
     </row>
     <row r="17">
@@ -4376,16 +4376,16 @@
         <v>40</v>
       </c>
       <c r="B17" t="n">
-        <v>364600.6336678743</v>
+        <v>386243.7045692179</v>
       </c>
       <c r="C17" t="n">
         <v>0</v>
       </c>
       <c r="D17" t="n">
-        <v>-104435.0126966651</v>
+        <v>-116747.6844486682</v>
       </c>
       <c r="E17" t="n">
-        <v>260165.6209712091</v>
+        <v>269496.0201205497</v>
       </c>
     </row>
     <row r="18">
@@ -4393,16 +4393,16 @@
         <v>41</v>
       </c>
       <c r="B18" t="n">
-        <v>433653.7839837595</v>
+        <v>454484.64177226</v>
       </c>
       <c r="C18" t="n">
         <v>0</v>
       </c>
       <c r="D18" t="n">
-        <v>-110053.6348546438</v>
+        <v>-127104.2915970053</v>
       </c>
       <c r="E18" t="n">
-        <v>323600.1491291157</v>
+        <v>327380.3501752546</v>
       </c>
     </row>
     <row r="19">
@@ -4410,16 +4410,16 @@
         <v>42</v>
       </c>
       <c r="B19" t="n">
-        <v>502706.9342996448</v>
+        <v>522725.578975302</v>
       </c>
       <c r="C19" t="n">
         <v>0</v>
       </c>
       <c r="D19" t="n">
-        <v>-114161.4651843996</v>
+        <v>-135981.8846414031</v>
       </c>
       <c r="E19" t="n">
-        <v>388545.4691152452</v>
+        <v>386743.694333899</v>
       </c>
     </row>
     <row r="20">
@@ -4427,16 +4427,16 @@
         <v>43</v>
       </c>
       <c r="B20" t="n">
-        <v>571760.0846155301</v>
+        <v>590966.516178344</v>
       </c>
       <c r="C20" t="n">
         <v>0</v>
       </c>
       <c r="D20" t="n">
-        <v>-117121.2836390998</v>
+        <v>-143562.8017719312</v>
       </c>
       <c r="E20" t="n">
-        <v>454638.8009764303</v>
+        <v>447403.7144064128</v>
       </c>
     </row>
     <row r="21">
@@ -4444,16 +4444,16 @@
         <v>44</v>
       </c>
       <c r="B21" t="n">
-        <v>640813.2349314153</v>
+        <v>659207.4533813862</v>
       </c>
       <c r="C21" t="n">
         <v>0</v>
       </c>
       <c r="D21" t="n">
-        <v>-119224.923500013</v>
+        <v>-150013.5556402022</v>
       </c>
       <c r="E21" t="n">
-        <v>521588.3114314022</v>
+        <v>509193.897741184</v>
       </c>
     </row>
     <row r="22">
@@ -4461,16 +4461,16 @@
         <v>45</v>
       </c>
       <c r="B22" t="n">
-        <v>709866.3852473006</v>
+        <v>727448.3905844283</v>
       </c>
       <c r="C22" t="n">
         <v>0</v>
       </c>
       <c r="D22" t="n">
-        <v>-120700.9708996238</v>
+        <v>-155484.5780323589</v>
       </c>
       <c r="E22" t="n">
-        <v>589165.4143476768</v>
+        <v>571963.8125520694</v>
       </c>
     </row>
     <row r="23">
@@ -4478,16 +4478,16 @@
         <v>46</v>
       </c>
       <c r="B23" t="n">
-        <v>778919.5355631858</v>
+        <v>795689.3277874703</v>
       </c>
       <c r="C23" t="n">
         <v>0</v>
       </c>
       <c r="D23" t="n">
-        <v>-121724.2736794409</v>
+        <v>-160110.4834128485</v>
       </c>
       <c r="E23" t="n">
-        <v>657195.2618837449</v>
+        <v>635578.8443746219</v>
       </c>
     </row>
     <row r="24">
@@ -4495,16 +4495,16 @@
         <v>47</v>
       </c>
       <c r="B24" t="n">
-        <v>847972.685879071</v>
+        <v>863930.2649905123</v>
       </c>
       <c r="C24" t="n">
         <v>0</v>
       </c>
       <c r="D24" t="n">
-        <v>-122425.7580211227</v>
+        <v>-164010.7134406035</v>
       </c>
       <c r="E24" t="n">
-        <v>725546.9278579484</v>
+        <v>699919.5515499087</v>
       </c>
     </row>
     <row r="25">
@@ -4512,16 +4512,16 @@
         <v>48</v>
       </c>
       <c r="B25" t="n">
-        <v>917025.8361949564</v>
+        <v>932171.2021935545</v>
       </c>
       <c r="C25" t="n">
         <v>0</v>
       </c>
       <c r="D25" t="n">
-        <v>-122901.5961791991</v>
+        <v>-167290.4443861627</v>
       </c>
       <c r="E25" t="n">
-        <v>794124.2400157574</v>
+        <v>764880.7578073918</v>
       </c>
     </row>
     <row r="26">
@@ -4529,16 +4529,16 @@
         <v>49</v>
       </c>
       <c r="B26" t="n">
-        <v>986078.9865108416</v>
+        <v>1000412.139396597</v>
       </c>
       <c r="C26" t="n">
         <v>0</v>
       </c>
       <c r="D26" t="n">
-        <v>-123221.2118366637</v>
+        <v>-170041.6598447259</v>
       </c>
       <c r="E26" t="n">
-        <v>862857.774674178</v>
+        <v>830370.4795518706</v>
       </c>
     </row>
     <row r="27">
@@ -4546,16 +4546,16 @@
         <v>50</v>
       </c>
       <c r="B27" t="n">
-        <v>1055132.136826727</v>
+        <v>1068653.076599639</v>
       </c>
       <c r="C27" t="n">
         <v>0</v>
       </c>
       <c r="D27" t="n">
-        <v>-123433.931337897</v>
+        <v>-172344.3107304194</v>
       </c>
       <c r="E27" t="n">
-        <v>931698.2054888298</v>
+        <v>896308.7658692192</v>
       </c>
     </row>
     <row r="28">
@@ -4563,16 +4563,16 @@
         <v>51</v>
       </c>
       <c r="B28" t="n">
-        <v>1124185.287142612</v>
+        <v>1136894.013802681</v>
       </c>
       <c r="C28" t="n">
         <v>0</v>
       </c>
       <c r="D28" t="n">
-        <v>-123574.2978568129</v>
+        <v>-174267.5023210493</v>
       </c>
       <c r="E28" t="n">
-        <v>1000610.989285799</v>
+        <v>962626.5114816313</v>
       </c>
     </row>
     <row r="29">
@@ -4580,16 +4580,16 @@
         <v>52</v>
       </c>
       <c r="B29" t="n">
-        <v>1193238.437458497</v>
+        <v>1205134.951005723</v>
       </c>
       <c r="C29" t="n">
         <v>0</v>
       </c>
       <c r="D29" t="n">
-        <v>-123666.1834407825</v>
+        <v>-175870.6636165766</v>
       </c>
       <c r="E29" t="n">
-        <v>1069572.254017715</v>
+        <v>1029264.287389146</v>
       </c>
     </row>
     <row r="30">
@@ -4597,16 +4597,16 @@
         <v>53</v>
       </c>
       <c r="B30" t="n">
-        <v>1262291.587774383</v>
+        <v>1273375.888208765</v>
       </c>
       <c r="C30" t="n">
         <v>0</v>
       </c>
       <c r="D30" t="n">
-        <v>-123725.8862048417</v>
+        <v>-177204.6673156105</v>
       </c>
       <c r="E30" t="n">
-        <v>1138565.701569541</v>
+        <v>1096171.220893154</v>
       </c>
     </row>
     <row r="31">
@@ -4614,16 +4614,16 @@
         <v>54</v>
       </c>
       <c r="B31" t="n">
-        <v>1331344.738090268</v>
+        <v>1341616.825411807</v>
       </c>
       <c r="C31" t="n">
         <v>0</v>
       </c>
       <c r="D31" t="n">
-        <v>-123764.4097263791</v>
+        <v>-178312.8793561657</v>
       </c>
       <c r="E31" t="n">
-        <v>1207580.328363889</v>
+        <v>1163303.946055641</v>
       </c>
     </row>
     <row r="32">
@@ -4631,16 +4631,16 @@
         <v>55</v>
       </c>
       <c r="B32" t="n">
-        <v>1400397.888406153</v>
+        <v>1409857.762614849</v>
       </c>
       <c r="C32" t="n">
         <v>0</v>
       </c>
       <c r="D32" t="n">
-        <v>-123789.107042558</v>
+        <v>-179232.1253977368</v>
       </c>
       <c r="E32" t="n">
-        <v>1276608.781363595</v>
+        <v>1230625.637217112</v>
       </c>
     </row>
     <row r="33">
@@ -4648,16 +4648,16 @@
         <v>56</v>
       </c>
       <c r="B33" t="n">
-        <v>1469451.038722039</v>
+        <v>1478098.699817891</v>
       </c>
       <c r="C33" t="n">
         <v>0</v>
       </c>
       <c r="D33" t="n">
-        <v>-123804.8454504178</v>
+        <v>-179993.5681017313</v>
       </c>
       <c r="E33" t="n">
-        <v>1345646.193271621</v>
+        <v>1298105.13171616</v>
       </c>
     </row>
     <row r="34">
@@ -4665,16 +4665,16 @@
         <v>57</v>
       </c>
       <c r="B34" t="n">
-        <v>1538504.189037924</v>
+        <v>1546339.637020933</v>
       </c>
       <c r="C34" t="n">
         <v>0</v>
       </c>
       <c r="D34" t="n">
-        <v>-123814.818824613</v>
+        <v>-180623.4938853296</v>
       </c>
       <c r="E34" t="n">
-        <v>1414689.370213311</v>
+        <v>1365716.143135604</v>
       </c>
     </row>
     <row r="35">
@@ -4682,16 +4682,16 @@
         <v>58</v>
       </c>
       <c r="B35" t="n">
-        <v>1607557.339353809</v>
+        <v>1614580.574223975</v>
       </c>
       <c r="C35" t="n">
         <v>0</v>
       </c>
       <c r="D35" t="n">
-        <v>-123821.1061436326</v>
+        <v>-181144.0112676926</v>
       </c>
       <c r="E35" t="n">
-        <v>1483736.233210176</v>
+        <v>1433436.562956283</v>
       </c>
     </row>
     <row r="36">
@@ -4699,16 +4699,16 @@
         <v>59</v>
       </c>
       <c r="B36" t="n">
-        <v>1676610.489669694</v>
+        <v>1682821.511427017</v>
       </c>
       <c r="C36" t="n">
         <v>0</v>
       </c>
       <c r="D36" t="n">
-        <v>-123825.0506456138</v>
+        <v>-181573.665265597</v>
       </c>
       <c r="E36" t="n">
-        <v>1552785.439024081</v>
+        <v>1501247.84616142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>